<commit_message>
Add updated presentation schedule
</commit_message>
<xml_diff>
--- a/presentation schedule.xlsx
+++ b/presentation schedule.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="24960" windowHeight="14740" tabRatio="500"/>
+    <workbookView xWindow="120" yWindow="460" windowWidth="16000" windowHeight="11460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>First Name</t>
   </si>
@@ -77,12 +77,6 @@
     <t xml:space="preserve">Ernst                         </t>
   </si>
   <si>
-    <t xml:space="preserve">Karri               </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Folks                         </t>
-  </si>
-  <si>
     <t xml:space="preserve">Ann                 </t>
   </si>
   <si>
@@ -141,6 +135,21 @@
   </si>
   <si>
     <t>Time</t>
+  </si>
+  <si>
+    <t>Andrew</t>
+  </si>
+  <si>
+    <t>Kaul</t>
+  </si>
+  <si>
+    <t>special</t>
+  </si>
+  <si>
+    <t>Karri</t>
+  </si>
+  <si>
+    <t>Folks</t>
   </si>
 </sst>
 </file>
@@ -466,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -485,21 +494,21 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -530,10 +539,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -547,10 +556,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -564,10 +573,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -615,10 +624,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -632,87 +641,87 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10">
-        <v>9</v>
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
       </c>
       <c r="D10" s="2">
-        <v>42710</v>
+        <v>42703</v>
       </c>
       <c r="E10" s="3">
-        <v>0.375</v>
+        <v>0.43055555555555558</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" s="2">
         <v>42710</v>
       </c>
       <c r="E11" s="3">
-        <v>0.38194444444444442</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D12" s="2">
         <v>42710</v>
       </c>
       <c r="E12" s="3">
-        <v>0.3888888888888889</v>
+        <v>0.38194444444444442</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D13" s="2">
         <v>42710</v>
       </c>
       <c r="E13" s="3">
-        <v>0.39583333333333298</v>
+        <v>0.3888888888888889</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D14" s="2">
         <v>42710</v>
       </c>
       <c r="E14" s="3">
-        <v>0.40277777777777801</v>
+        <v>0.39583333333333298</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -723,68 +732,85 @@
         <v>21</v>
       </c>
       <c r="C15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D15" s="2">
         <v>42710</v>
       </c>
       <c r="E15" s="3">
-        <v>0.40972222222222199</v>
+        <v>0.40277777777777801</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="C16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D16" s="2">
         <v>42710</v>
       </c>
       <c r="E16" s="3">
-        <v>0.41666666666666702</v>
+        <v>0.40972222222222199</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="C17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D17" s="2">
         <v>42710</v>
       </c>
       <c r="E17" s="3">
-        <v>0.42361111111111099</v>
+        <v>0.41666666666666702</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D18" s="2">
         <v>42710</v>
       </c>
       <c r="E18" s="3">
+        <v>0.42361111111111099</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19">
+        <v>17</v>
+      </c>
+      <c r="D19" s="2">
+        <v>42710</v>
+      </c>
+      <c r="E19" s="3">
         <v>0.43055555555555503</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E19" s="3"/>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E20" s="3"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:F1">

</xml_diff>